<commit_message>
Minute updates for training.
</commit_message>
<xml_diff>
--- a/Timeline.xlsx
+++ b/Timeline.xlsx
@@ -78,13 +78,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -95,7 +101,14 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -107,7 +120,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -115,7 +128,13 @@
     <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
   </cellXfs>
@@ -426,20 +445,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="28.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="3" width="14.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="3" width="22.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="4" width="28.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="5" width="14.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="22.433571428571426" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -450,106 +469,122 @@
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="3">
         <v>45207</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="3">
         <v>45213</v>
       </c>
-      <c r="D2" s="1"/>
+      <c r="D2" s="2">
+        <v>45219</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="3">
         <v>45214</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="3">
         <v>45227</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="D3" s="2">
+        <v>45240</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="3">
         <v>45228</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="3">
         <v>45241</v>
       </c>
-      <c r="D4" s="1"/>
+      <c r="D4" s="2">
+        <v>45250</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="3">
         <v>45242</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="3">
         <v>45255</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="D5" s="2">
+        <v>45250</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="3">
         <v>45256</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="3">
         <v>45283</v>
       </c>
-      <c r="D6" s="1"/>
+      <c r="D6" s="2">
+        <v>45252</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="3">
         <v>45284</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="3">
         <v>45304</v>
       </c>
-      <c r="D7" s="1"/>
+      <c r="D7" s="2">
+        <v>45252</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="3">
         <v>45305</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="3">
         <v>45318</v>
       </c>
-      <c r="D8" s="1"/>
+      <c r="D8" s="2">
+        <v>45254</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="3">
         <v>45319</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="3">
         <v>45325</v>
       </c>
-      <c r="D9" s="1"/>
+      <c r="D9" s="2">
+        <v>45255</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="3">
         <v>45326</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="3">
         <v>45332</v>
       </c>
       <c r="D10" s="1"/>
@@ -558,10 +593,10 @@
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="3">
         <v>45333</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="3">
         <v>45339</v>
       </c>
       <c r="D11" s="1"/>
@@ -570,10 +605,10 @@
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="3">
         <v>45340</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="3">
         <v>45353</v>
       </c>
       <c r="D12" s="1"/>
@@ -582,10 +617,10 @@
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="3">
         <v>45354</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="3">
         <v>45367</v>
       </c>
       <c r="D13" s="1"/>
@@ -594,10 +629,10 @@
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="3">
         <v>45368</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="3">
         <v>45395</v>
       </c>
       <c r="D14" s="1"/>
@@ -606,10 +641,10 @@
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="3">
         <v>45207</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="3">
         <v>45395</v>
       </c>
       <c r="D15" s="1"/>
@@ -618,10 +653,10 @@
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="3">
         <v>45382</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="3">
         <v>45395</v>
       </c>
       <c r="D16" s="1"/>

</xml_diff>